<commit_message>
Validazione preliminari input files
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Ran Rate.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Ran Rate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,54 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,13 +64,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -44,14 +99,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +198,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +406,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.05</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>